<commit_message>
adding new display template, changing store display count
</commit_message>
<xml_diff>
--- a/Projects/PEPSICORU/Data/Template.xlsx
+++ b/Projects/PEPSICORU/Data/Template.xlsx
@@ -14,7 +14,6 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$148</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$148</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$H$148</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$H$148</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1158,22 +1157,25 @@
   <dimension ref="A1:H148"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.7959183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.3367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="65.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1199,7 +1201,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -1213,7 +1215,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -1229,7 +1231,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1245,16 +1247,14 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="4" t="n">
         <v>2</v>
       </c>
@@ -1265,16 +1265,14 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4" t="n">
-        <v>2</v>
-      </c>
+      <c r="C6" s="4"/>
       <c r="D6" s="4" t="n">
         <v>2</v>
       </c>
@@ -1285,7 +1283,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -1301,7 +1299,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -1319,7 +1317,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
@@ -1337,7 +1335,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -1351,7 +1349,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -1367,7 +1365,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>28</v>
       </c>
@@ -1381,7 +1379,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>30</v>
       </c>
@@ -1399,7 +1397,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -1415,7 +1413,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>34</v>
       </c>
@@ -1433,16 +1431,14 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="C16" s="4"/>
       <c r="D16" s="4" t="n">
         <v>2</v>
       </c>
@@ -1455,7 +1451,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>38</v>
       </c>
@@ -1473,7 +1469,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>40</v>
       </c>
@@ -1491,7 +1487,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
@@ -1511,7 +1507,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
         <v>44</v>
       </c>
@@ -1525,16 +1521,14 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="C21" s="4"/>
       <c r="D21" s="4" t="n">
         <v>2</v>
       </c>
@@ -1547,7 +1541,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
         <v>48</v>
       </c>
@@ -1563,7 +1557,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
         <v>50</v>
       </c>
@@ -1581,16 +1575,14 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="C24" s="4"/>
       <c r="D24" s="4" t="n">
         <v>2</v>
       </c>
@@ -1603,16 +1595,14 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="C25" s="4"/>
       <c r="D25" s="4" t="n">
         <v>1</v>
       </c>
@@ -1623,16 +1613,14 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="4" t="n">
         <v>1</v>
       </c>
@@ -1643,7 +1631,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
         <v>58</v>
       </c>
@@ -1661,16 +1649,14 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="C28" s="4"/>
       <c r="D28" s="4" t="n">
         <v>2</v>
       </c>
@@ -1683,16 +1669,14 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="C29" s="4"/>
       <c r="D29" s="4" t="n">
         <v>1</v>
       </c>
@@ -1703,16 +1687,14 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
         <v>64</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="C30" s="4"/>
       <c r="D30" s="4" t="n">
         <v>1</v>
       </c>
@@ -1725,16 +1707,14 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="C31" s="4"/>
       <c r="D31" s="4" t="n">
         <v>1</v>
       </c>
@@ -1747,16 +1727,14 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="4" t="n">
-        <v>2</v>
-      </c>
+      <c r="C32" s="4"/>
       <c r="D32" s="4" t="n">
         <v>2</v>
       </c>
@@ -1769,7 +1747,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
         <v>70</v>
       </c>
@@ -1787,7 +1765,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
         <v>72</v>
       </c>
@@ -1805,16 +1783,14 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="C35" s="4"/>
       <c r="D35" s="4" t="n">
         <v>2</v>
       </c>
@@ -1825,7 +1801,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
         <v>76</v>
       </c>
@@ -1843,7 +1819,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
         <v>78</v>
       </c>
@@ -1859,16 +1835,14 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="C38" s="4"/>
       <c r="D38" s="4" t="n">
         <v>2</v>
       </c>
@@ -1879,16 +1853,14 @@
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
         <v>82</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="C39" s="4"/>
       <c r="D39" s="4" t="n">
         <v>1</v>
       </c>
@@ -1899,16 +1871,14 @@
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
         <v>84</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="C40" s="4"/>
       <c r="D40" s="4" t="n">
         <v>2</v>
       </c>
@@ -1919,7 +1889,7 @@
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
         <v>86</v>
       </c>
@@ -1939,7 +1909,7 @@
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
         <v>88</v>
       </c>
@@ -1955,7 +1925,7 @@
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
         <v>90</v>
       </c>
@@ -1971,16 +1941,14 @@
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
         <v>92</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="4" t="n">
-        <v>2</v>
-      </c>
+      <c r="C44" s="4"/>
       <c r="D44" s="4" t="n">
         <v>2</v>
       </c>
@@ -1991,7 +1959,7 @@
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
         <v>94</v>
       </c>
@@ -2009,7 +1977,7 @@
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
         <v>96</v>
       </c>
@@ -2023,7 +1991,7 @@
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
         <v>98</v>
       </c>
@@ -2037,7 +2005,7 @@
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
         <v>100</v>
       </c>
@@ -2051,16 +2019,14 @@
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C49" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="C49" s="4"/>
       <c r="D49" s="4" t="n">
         <v>1</v>
       </c>
@@ -2071,7 +2037,7 @@
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
         <v>104</v>
       </c>
@@ -2087,7 +2053,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
         <v>106</v>
       </c>
@@ -2105,7 +2071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
         <v>108</v>
       </c>
@@ -2123,7 +2089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
         <v>110</v>
       </c>
@@ -2141,7 +2107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
         <v>112</v>
       </c>
@@ -2159,14 +2125,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
         <v>114</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C55" s="4"/>
+      <c r="C55" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
@@ -2177,7 +2145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
         <v>116</v>
       </c>
@@ -2195,7 +2163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
         <v>118</v>
       </c>
@@ -2213,7 +2181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
         <v>120</v>
       </c>
@@ -2229,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
         <v>122</v>
       </c>
@@ -2247,7 +2215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
         <v>124</v>
       </c>
@@ -2265,7 +2233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
         <v>126</v>
       </c>
@@ -2283,14 +2251,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
         <v>128</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C62" s="4"/>
+      <c r="C62" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
@@ -2301,7 +2271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
         <v>130</v>
       </c>
@@ -2319,14 +2289,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
         <v>132</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C64" s="4"/>
+      <c r="C64" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
@@ -2337,7 +2309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
         <v>134</v>
       </c>
@@ -2355,14 +2327,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
         <v>136</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C66" s="4"/>
+      <c r="C66" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
@@ -2373,14 +2347,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="s">
         <v>138</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C67" s="4"/>
+      <c r="C67" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
@@ -2389,14 +2365,16 @@
       </c>
       <c r="H67" s="4"/>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
         <v>140</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C68" s="4"/>
+      <c r="C68" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
@@ -2407,7 +2385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
         <v>142</v>
       </c>
@@ -2425,14 +2403,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
         <v>144</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C70" s="4"/>
+      <c r="C70" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
@@ -2443,14 +2423,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
         <v>146</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C71" s="4"/>
+      <c r="C71" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
@@ -2461,14 +2443,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
         <v>148</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C72" s="4"/>
+      <c r="C72" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
@@ -2479,14 +2463,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="s">
         <v>150</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C73" s="4"/>
+      <c r="C73" s="4" t="n">
+        <v>2</v>
+      </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
@@ -2497,14 +2483,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="s">
         <v>152</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C74" s="4"/>
+      <c r="C74" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
@@ -2515,14 +2503,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
         <v>154</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C75" s="4"/>
+      <c r="C75" s="4" t="n">
+        <v>2</v>
+      </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
@@ -2533,7 +2523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="s">
         <v>156</v>
       </c>
@@ -2551,7 +2541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="s">
         <v>158</v>
       </c>
@@ -2569,14 +2559,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="s">
         <v>160</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C78" s="4"/>
+      <c r="C78" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
@@ -2587,7 +2579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
         <v>162</v>
       </c>
@@ -2605,7 +2597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="4" t="s">
         <v>164</v>
       </c>
@@ -2623,14 +2615,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="s">
         <v>166</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C81" s="4"/>
+      <c r="C81" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
@@ -2641,14 +2635,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C82" s="4"/>
+      <c r="C82" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
@@ -2659,7 +2655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="s">
         <v>170</v>
       </c>
@@ -2677,14 +2673,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="s">
         <v>172</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C84" s="4"/>
+      <c r="C84" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
@@ -2695,7 +2693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
         <v>174</v>
       </c>
@@ -2713,7 +2711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="4" t="s">
         <v>176</v>
       </c>
@@ -2731,7 +2729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="s">
         <v>178</v>
       </c>
@@ -2749,7 +2747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="s">
         <v>180</v>
       </c>
@@ -2763,14 +2761,16 @@
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="4" t="s">
         <v>182</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C89" s="4"/>
+      <c r="C89" s="4" t="n">
+        <v>2</v>
+      </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
@@ -2781,7 +2781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="4" t="s">
         <v>184</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="4" t="s">
         <v>186</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="4" t="s">
         <v>188</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="4" t="s">
         <v>190</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="4" t="s">
         <v>192</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="4" t="s">
         <v>194</v>
       </c>
@@ -2885,7 +2885,7 @@
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="4" t="s">
         <v>196</v>
       </c>
@@ -2903,14 +2903,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
         <v>198</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C97" s="4"/>
+      <c r="C97" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
@@ -2919,7 +2921,7 @@
       </c>
       <c r="H97" s="4"/>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="4" t="s">
         <v>200</v>
       </c>
@@ -2933,7 +2935,7 @@
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="4" t="s">
         <v>202</v>
       </c>
@@ -2947,7 +2949,7 @@
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="4" t="s">
         <v>204</v>
       </c>
@@ -2967,7 +2969,7 @@
       </c>
       <c r="H100" s="4"/>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="4" t="s">
         <v>206</v>
       </c>
@@ -2989,7 +2991,7 @@
       </c>
       <c r="H101" s="4"/>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="4" t="s">
         <v>208</v>
       </c>
@@ -3011,7 +3013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="4" t="s">
         <v>210</v>
       </c>
@@ -3027,7 +3029,7 @@
       </c>
       <c r="H103" s="4"/>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="4" t="s">
         <v>212</v>
       </c>
@@ -3053,7 +3055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="4" t="s">
         <v>214</v>
       </c>
@@ -3079,7 +3081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="4" t="s">
         <v>216</v>
       </c>
@@ -3105,7 +3107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="4" t="s">
         <v>218</v>
       </c>
@@ -3127,7 +3129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="4" t="s">
         <v>220</v>
       </c>
@@ -3145,7 +3147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="4" t="s">
         <v>222</v>
       </c>
@@ -3167,7 +3169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="4" t="s">
         <v>224</v>
       </c>
@@ -3189,7 +3191,7 @@
       </c>
       <c r="H110" s="4"/>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="4" t="s">
         <v>226</v>
       </c>
@@ -3213,7 +3215,7 @@
       </c>
       <c r="H111" s="4"/>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="4" t="s">
         <v>228</v>
       </c>
@@ -3237,7 +3239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="4" t="s">
         <v>230</v>
       </c>
@@ -3255,7 +3257,7 @@
       </c>
       <c r="H113" s="4"/>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="4" t="s">
         <v>232</v>
       </c>
@@ -3279,7 +3281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="4" t="s">
         <v>234</v>
       </c>
@@ -3297,7 +3299,7 @@
       </c>
       <c r="H115" s="4"/>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="4" t="s">
         <v>236</v>
       </c>
@@ -3317,7 +3319,7 @@
       </c>
       <c r="H116" s="4"/>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="4" t="s">
         <v>238</v>
       </c>
@@ -3339,7 +3341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="4" t="s">
         <v>240</v>
       </c>
@@ -3359,7 +3361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="4" t="s">
         <v>242</v>
       </c>
@@ -3379,7 +3381,7 @@
       </c>
       <c r="H119" s="4"/>
     </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="4" t="s">
         <v>244</v>
       </c>
@@ -3405,7 +3407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="4" t="s">
         <v>246</v>
       </c>
@@ -3427,7 +3429,7 @@
       </c>
       <c r="H121" s="4"/>
     </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="4" t="s">
         <v>248</v>
       </c>
@@ -3453,7 +3455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="4" t="s">
         <v>250</v>
       </c>
@@ -3475,7 +3477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="4" t="s">
         <v>252</v>
       </c>
@@ -3493,7 +3495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="4" t="s">
         <v>254</v>
       </c>
@@ -3513,7 +3515,7 @@
       </c>
       <c r="H125" s="4"/>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="4" t="s">
         <v>256</v>
       </c>
@@ -3537,7 +3539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="4" t="s">
         <v>258</v>
       </c>
@@ -3559,7 +3561,7 @@
       </c>
       <c r="H127" s="4"/>
     </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="4" t="s">
         <v>260</v>
       </c>
@@ -3575,7 +3577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="4" t="s">
         <v>262</v>
       </c>
@@ -3599,7 +3601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="4" t="s">
         <v>264</v>
       </c>
@@ -3615,7 +3617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="4" t="s">
         <v>266</v>
       </c>
@@ -3639,7 +3641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="4" t="s">
         <v>268</v>
       </c>
@@ -3659,7 +3661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="4" t="s">
         <v>270</v>
       </c>
@@ -3681,7 +3683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="4" t="s">
         <v>272</v>
       </c>
@@ -3705,7 +3707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="4" t="s">
         <v>274</v>
       </c>
@@ -3721,7 +3723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="4" t="s">
         <v>276</v>
       </c>
@@ -3743,7 +3745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="4" t="s">
         <v>278</v>
       </c>
@@ -3761,7 +3763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="4" t="s">
         <v>280</v>
       </c>
@@ -3777,7 +3779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="4" t="s">
         <v>282</v>
       </c>
@@ -3795,7 +3797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="4" t="s">
         <v>284</v>
       </c>
@@ -3819,7 +3821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="4" t="s">
         <v>286</v>
       </c>
@@ -3837,7 +3839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="4" t="s">
         <v>288</v>
       </c>
@@ -3853,7 +3855,7 @@
       <c r="G142" s="4"/>
       <c r="H142" s="4"/>
     </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="4" t="s">
         <v>290</v>
       </c>
@@ -3873,7 +3875,7 @@
       <c r="G143" s="4"/>
       <c r="H143" s="4"/>
     </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="4" t="s">
         <v>292</v>
       </c>
@@ -3889,7 +3891,7 @@
       <c r="G144" s="4"/>
       <c r="H144" s="4"/>
     </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="4" t="s">
         <v>294</v>
       </c>
@@ -3907,7 +3909,7 @@
       <c r="G145" s="4"/>
       <c r="H145" s="4"/>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="4" t="s">
         <v>296</v>
       </c>
@@ -3921,7 +3923,7 @@
       <c r="G146" s="4"/>
       <c r="H146" s="4"/>
     </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="4" t="s">
         <v>298</v>
       </c>
@@ -3947,7 +3949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="4" t="s">
         <v>300</v>
       </c>

</xml_diff>